<commit_message>
non-gradient local search development
local search algorithm, updates to launch and development costs modules,
and attempt at using fminsearch
</commit_message>
<xml_diff>
--- a/MSDO/Assignment3/LocalNonGradientSearchSummary.xlsx
+++ b/MSDO/Assignment3/LocalNonGradientSearchSummary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="60">
   <si>
     <t>Starting Point</t>
   </si>
@@ -163,6 +163,39 @@
   </si>
   <si>
     <t>[5,1,0,0,0]</t>
+  </si>
+  <si>
+    <t>LAUNCH COST SENSITIVITY STUDY</t>
+  </si>
+  <si>
+    <t>Launch Cost ($/kg)</t>
+  </si>
+  <si>
+    <t>[3,1,2,2,1]</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>[0,1,0,0,0]</t>
+  </si>
+  <si>
+    <t># of Missions</t>
+  </si>
+  <si>
+    <t>NUMBER OF MISSIONS SENSITIVITY STUDY</t>
+  </si>
+  <si>
+    <t>Global Maximum</t>
+  </si>
+  <si>
+    <t>Local Maximums (darker is worse)</t>
+  </si>
+  <si>
+    <t>[2,1,0,0,0]</t>
+  </si>
+  <si>
+    <t>[6,1,0,0,0]</t>
   </si>
 </sst>
 </file>
@@ -280,10 +313,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -325,6 +361,15 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1433,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:M41"/>
+  <dimension ref="A4:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,225 +1499,225 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>2.6639E-5</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>4</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>18</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="14">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>2.6639E-5</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <v>7</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>43</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="15">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>1.7640999999999999E-5</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="5">
         <v>8</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
         <v>45</v>
       </c>
       <c r="H7" s="2">
         <v>2</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J7" s="2"/>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="12">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <v>1.7640999999999999E-5</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="5">
         <v>7</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="5">
         <v>43</v>
       </c>
       <c r="H8" s="2">
         <v>3</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="15" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="2"/>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="15" t="s">
         <v>39</v>
       </c>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <v>2.6639E-5</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="5">
         <v>10</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="5">
         <v>64</v>
       </c>
       <c r="H9" s="2">
         <v>4</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="12" t="s">
         <v>23</v>
       </c>
       <c r="J9" s="2"/>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <v>3.3074000000000002E-5</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="5">
         <v>8</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="5">
         <v>48</v>
       </c>
       <c r="H10" s="2">
         <v>5</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="15" t="s">
         <v>24</v>
       </c>
       <c r="J10" s="2"/>
@@ -1681,25 +1726,25 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="6">
         <v>3.3074000000000002E-5</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="5">
         <v>9</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="5">
         <v>62</v>
       </c>
       <c r="H11" s="2">
         <v>6</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="12" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="2"/>
@@ -1708,61 +1753,70 @@
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>2.5004E-5</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="5">
         <v>4</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="5">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="6">
         <v>2.5004E-5</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="5">
         <v>7</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="5">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="6">
         <v>3.3074000000000002E-5</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="5">
         <v>9</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="5">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I15" s="15">
+      <c r="B15" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="I15" s="16">
         <v>2.6461999999999998E-5</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="16">
         <v>2.6461999999999998E-5</v>
       </c>
       <c r="K15" s="1">
@@ -1776,10 +1830,10 @@
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I16" s="15">
+      <c r="I16" s="16">
         <v>2.6639E-5</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="16">
         <v>2.6461E-5</v>
       </c>
       <c r="K16" s="1">
@@ -1793,7 +1847,7 @@
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I17" s="15">
+      <c r="I17" s="16">
         <v>2.6495999999999998E-5</v>
       </c>
       <c r="K17" s="1">
@@ -1807,7 +1861,7 @@
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I18" s="15">
+      <c r="I18" s="16">
         <v>2.4890999999999999E-5</v>
       </c>
       <c r="K18" s="1">
@@ -1818,7 +1872,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I19" s="15">
+      <c r="I19" s="16">
         <v>1.7091999999999998E-5</v>
       </c>
       <c r="K19" s="1">
@@ -1829,12 +1883,12 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I20" s="15">
+      <c r="I20" s="16">
         <v>1.7640999999999999E-5</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I21" s="15">
+      <c r="I21" s="16">
         <v>1.7583000000000001E-5</v>
       </c>
     </row>
@@ -1844,155 +1898,164 @@
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H34" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I34" s="10" t="s">
+      <c r="I34" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J34" s="10" t="s">
+      <c r="J34" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K34" s="10" t="s">
+      <c r="K34" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L34" s="10" t="s">
+      <c r="L34" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="M34" s="10" t="s">
+      <c r="M34" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="6">
         <v>3.3074000000000002E-5</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="5">
         <v>5</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="5">
         <v>24</v>
       </c>
       <c r="H35" s="2">
         <v>0</v>
       </c>
-      <c r="I35" s="12" t="s">
+      <c r="I35" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="14" t="s">
+      <c r="J35" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="K35" s="13" t="s">
+      <c r="K35" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="L35" s="13" t="s">
+      <c r="L35" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="M35" s="13">
+      <c r="M35" s="14">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="6">
         <v>3.3074000000000002E-5</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="5">
         <v>15</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="5">
         <v>98</v>
       </c>
       <c r="H36" s="2">
         <v>1</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="I36" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="14" t="s">
+      <c r="J36" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="K36" s="14" t="s">
+      <c r="K36" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="L36" s="14" t="s">
+      <c r="L36" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="M36" s="14">
+      <c r="M36" s="15">
         <v>18</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="6">
         <v>2.19E-5</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="5">
         <v>14</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="5">
         <v>80</v>
       </c>
       <c r="H37" s="2">
         <v>2</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="I37" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J37" s="2"/>
-      <c r="K37" s="12" t="s">
+      <c r="K37" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="L37" s="12" t="s">
+      <c r="L37" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="M37" s="11">
+      <c r="M37" s="12">
         <v>12</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
       <c r="H38" s="2">
         <v>3</v>
       </c>
-      <c r="I38" s="14" t="s">
+      <c r="I38" s="15" t="s">
         <v>22</v>
       </c>
       <c r="J38" s="2"/>
-      <c r="K38" s="11" t="s">
+      <c r="K38" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="L38" s="11" t="s">
+      <c r="L38" s="12" t="s">
         <v>39</v>
       </c>
       <c r="M38" s="2"/>
@@ -2001,14 +2064,14 @@
       <c r="H39" s="2">
         <v>4</v>
       </c>
-      <c r="I39" s="11" t="s">
+      <c r="I39" s="12" t="s">
         <v>23</v>
       </c>
       <c r="J39" s="2"/>
-      <c r="K39" s="11" t="s">
+      <c r="K39" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L39" s="11" t="s">
+      <c r="L39" s="12" t="s">
         <v>37</v>
       </c>
       <c r="M39" s="2"/>
@@ -2017,7 +2080,7 @@
       <c r="H40" s="2">
         <v>5</v>
       </c>
-      <c r="I40" s="14" t="s">
+      <c r="I40" s="15" t="s">
         <v>24</v>
       </c>
       <c r="J40" s="2"/>
@@ -2029,7 +2092,7 @@
       <c r="H41" s="2">
         <v>6</v>
       </c>
-      <c r="I41" s="11" t="s">
+      <c r="I41" s="12" t="s">
         <v>25</v>
       </c>
       <c r="J41" s="2"/>
@@ -2037,7 +2100,660 @@
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
     </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+      <c r="I49" t="s">
+        <v>50</v>
+      </c>
+      <c r="K49" t="s">
+        <v>1</v>
+      </c>
+      <c r="M49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I50" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L50" s="2"/>
+      <c r="M50" s="3">
+        <v>3.3074000000000002E-5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="6">
+        <v>3.3074000000000002E-5</v>
+      </c>
+      <c r="E51" s="5">
+        <v>5</v>
+      </c>
+      <c r="F51" s="5">
+        <v>24</v>
+      </c>
+      <c r="I51" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L51" s="2"/>
+      <c r="M51" s="3">
+        <v>3.3074000000000002E-5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" s="6">
+        <v>3.3074000000000002E-5</v>
+      </c>
+      <c r="E52" s="5">
+        <v>10</v>
+      </c>
+      <c r="F52" s="5">
+        <v>65</v>
+      </c>
+      <c r="I52" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L52" s="2"/>
+      <c r="M52" s="3">
+        <v>2.19E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="6">
+        <v>2.19E-5</v>
+      </c>
+      <c r="E53" s="5">
+        <v>14</v>
+      </c>
+      <c r="F53" s="5">
+        <v>80</v>
+      </c>
+      <c r="I53" s="2">
+        <v>7140</v>
+      </c>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L53" s="2"/>
+      <c r="M53" s="3">
+        <v>4.5979000000000001E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="20">
+        <v>7140</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D54" s="6">
+        <v>4.5979000000000001E-5</v>
+      </c>
+      <c r="E54" s="5">
+        <v>5</v>
+      </c>
+      <c r="F54" s="5">
+        <v>24</v>
+      </c>
+      <c r="I54" s="2">
+        <v>7140</v>
+      </c>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L54" s="2"/>
+      <c r="M54" s="3">
+        <v>4.5969E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="20">
+        <v>7140</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D55" s="6">
+        <v>4.5969E-5</v>
+      </c>
+      <c r="E55" s="5">
+        <v>10</v>
+      </c>
+      <c r="F55" s="5">
+        <v>66</v>
+      </c>
+      <c r="I55" s="2">
+        <v>7140</v>
+      </c>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L55" s="2"/>
+      <c r="M55" s="3">
+        <v>2.9509000000000002E-5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="20">
+        <v>7140</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D56" s="6">
+        <v>2.9509000000000002E-5</v>
+      </c>
+      <c r="E56" s="5">
+        <v>14</v>
+      </c>
+      <c r="F56" s="5">
+        <v>80</v>
+      </c>
+      <c r="I56" s="2">
+        <v>1600</v>
+      </c>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L56" s="2"/>
+      <c r="M56" s="3">
+        <v>1.9023E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="20">
+        <v>1600</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57" s="6">
+        <v>1.9023E-4</v>
+      </c>
+      <c r="E57" s="5">
+        <v>4</v>
+      </c>
+      <c r="F57" s="5">
+        <v>16</v>
+      </c>
+      <c r="I57" s="2">
+        <v>1600</v>
+      </c>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L57" s="2"/>
+      <c r="M57" s="3">
+        <v>1.9023E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="20">
+        <v>1600</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D58" s="6">
+        <v>1.9023E-4</v>
+      </c>
+      <c r="E58" s="5">
+        <v>11</v>
+      </c>
+      <c r="F58" s="5">
+        <v>73</v>
+      </c>
+      <c r="I58" s="2">
+        <v>1600</v>
+      </c>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L58" s="2"/>
+      <c r="M58" s="3">
+        <v>1.9023E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="20">
+        <v>1600</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D59" s="6">
+        <v>1.9023E-4</v>
+      </c>
+      <c r="E59" s="5">
+        <v>19</v>
+      </c>
+      <c r="F59" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B60" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="18"/>
+      <c r="D60" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>55</v>
+      </c>
+      <c r="I65" t="s">
+        <v>54</v>
+      </c>
+      <c r="K65" t="s">
+        <v>1</v>
+      </c>
+      <c r="M65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I66" s="2">
+        <v>10</v>
+      </c>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L66" s="2"/>
+      <c r="M66" s="3">
+        <v>3.3074000000000002E-5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="20">
+        <v>10</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D67" s="6">
+        <v>3.3074000000000002E-5</v>
+      </c>
+      <c r="E67" s="5">
+        <v>5</v>
+      </c>
+      <c r="F67" s="5">
+        <v>24</v>
+      </c>
+      <c r="I67" s="2">
+        <v>10</v>
+      </c>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L67" s="2"/>
+      <c r="M67" s="3">
+        <v>3.3074000000000002E-5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="20">
+        <v>10</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D68" s="6">
+        <v>3.3074000000000002E-5</v>
+      </c>
+      <c r="E68" s="5">
+        <v>10</v>
+      </c>
+      <c r="F68" s="5">
+        <v>65</v>
+      </c>
+      <c r="I68" s="2">
+        <v>10</v>
+      </c>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L68" s="2"/>
+      <c r="M68" s="3">
+        <v>2.19E-5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="20">
+        <v>10</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D69" s="6">
+        <v>2.19E-5</v>
+      </c>
+      <c r="E69" s="5">
+        <v>14</v>
+      </c>
+      <c r="F69" s="5">
+        <v>80</v>
+      </c>
+      <c r="I69" s="2">
+        <v>5</v>
+      </c>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L69" s="2"/>
+      <c r="M69" s="3">
+        <v>3.2468999999999997E-5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="20">
+        <v>5</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D70" s="6">
+        <v>3.2468999999999997E-5</v>
+      </c>
+      <c r="E70" s="5">
+        <v>5</v>
+      </c>
+      <c r="F70" s="5">
+        <v>24</v>
+      </c>
+      <c r="I70" s="2">
+        <v>5</v>
+      </c>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L70" s="2"/>
+      <c r="M70" s="3">
+        <v>3.2468999999999997E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="20">
+        <v>5</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D71" s="6">
+        <v>3.2468999999999997E-5</v>
+      </c>
+      <c r="E71" s="5">
+        <v>10</v>
+      </c>
+      <c r="F71" s="5">
+        <v>66</v>
+      </c>
+      <c r="I71" s="2">
+        <v>5</v>
+      </c>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L71" s="2"/>
+      <c r="M71" s="3">
+        <v>1.9938000000000001E-5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="20">
+        <v>5</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D72" s="6">
+        <v>1.9938000000000001E-5</v>
+      </c>
+      <c r="E72" s="5">
+        <v>14</v>
+      </c>
+      <c r="F72" s="5">
+        <v>80</v>
+      </c>
+      <c r="I72" s="2">
+        <v>15</v>
+      </c>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L72" s="2"/>
+      <c r="M72" s="3">
+        <v>3.3352999999999997E-5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="20">
+        <v>15</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D73" s="6">
+        <v>3.3352999999999997E-5</v>
+      </c>
+      <c r="E73" s="5">
+        <v>6</v>
+      </c>
+      <c r="F73" s="5">
+        <v>30</v>
+      </c>
+      <c r="I73" s="2">
+        <v>15</v>
+      </c>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L73" s="2"/>
+      <c r="M73" s="3">
+        <v>3.3352999999999997E-5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="20">
+        <v>15</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D74" s="6">
+        <v>3.3352999999999997E-5</v>
+      </c>
+      <c r="E74" s="5">
+        <v>9</v>
+      </c>
+      <c r="F74" s="5">
+        <v>59</v>
+      </c>
+      <c r="I74" s="2">
+        <v>15</v>
+      </c>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L74" s="2"/>
+      <c r="M74" s="3">
+        <v>2.2751999999999998E-5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="20">
+        <v>15</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D75" s="6">
+        <v>2.2751999999999998E-5</v>
+      </c>
+      <c r="E75" s="5">
+        <v>13</v>
+      </c>
+      <c r="F75" s="5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="20"/>
+      <c r="B76" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" s="18"/>
+      <c r="D76" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+    </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:F60"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Updated assignment with Part B3 done.
parker dropped in text and pictures for B3 ii and iii
</commit_message>
<xml_diff>
--- a/MSDO/Assignment3/LocalNonGradientSearchSummary.xlsx
+++ b/MSDO/Assignment3/LocalNonGradientSearchSummary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="60">
   <si>
     <t>Starting Point</t>
   </si>
@@ -203,7 +203,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -313,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -358,9 +358,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -368,9 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,11 +509,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="55144448"/>
-        <c:axId val="55122176"/>
+        <c:axId val="136663040"/>
+        <c:axId val="136664576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55144448"/>
+        <c:axId val="136663040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -523,12 +524,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55122176"/>
+        <c:crossAx val="136664576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55122176"/>
+        <c:axId val="136664576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,7 +558,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55144448"/>
+        <c:crossAx val="136663040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -674,11 +675,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="55624448"/>
-        <c:axId val="55625984"/>
+        <c:axId val="136680960"/>
+        <c:axId val="136682496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55624448"/>
+        <c:axId val="136680960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -689,12 +690,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55625984"/>
+        <c:crossAx val="136682496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55625984"/>
+        <c:axId val="136682496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,7 +724,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55624448"/>
+        <c:crossAx val="136680960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -840,11 +841,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72727936"/>
-        <c:axId val="61939712"/>
+        <c:axId val="136707072"/>
+        <c:axId val="137765632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72727936"/>
+        <c:axId val="136707072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -855,12 +856,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61939712"/>
+        <c:crossAx val="137765632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61939712"/>
+        <c:axId val="137765632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,7 +890,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72727936"/>
+        <c:crossAx val="136707072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -994,11 +995,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63408000"/>
-        <c:axId val="63419520"/>
+        <c:axId val="137810688"/>
+        <c:axId val="137812224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63408000"/>
+        <c:axId val="137810688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -1009,12 +1010,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63419520"/>
+        <c:crossAx val="137812224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63419520"/>
+        <c:axId val="137812224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1043,7 +1044,435 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63408000"/>
+        <c:crossAx val="137810688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Launch Cost</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> Sensitivity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.32250159741268297"/>
+          <c:y val="0.28256433663528624"/>
+          <c:w val="0.55927138321192993"/>
+          <c:h val="0.42678643748612888"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.1329334394998378"/>
+                  <c:y val="-0.24124017355442598"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$50:$O$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7140</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$50:$Q$52</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.3074000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5979000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9023E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="32911744"/>
+        <c:axId val="32917376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="32911744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Launch Cost</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> ($/kg)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="32917376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="32917376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Value</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (science/$M)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="32911744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Mission No.</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t>  Sensitivity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.28192711866072923"/>
+          <c:y val="0.28256433663528624"/>
+          <c:w val="0.65415278146411471"/>
+          <c:h val="0.4875651831109265"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.2945923894344665E-2"/>
+                  <c:y val="-0.13061747257329193"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$66:$O$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$66:$Q$68</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.2468999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3074000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3352999999999997E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="68792704"/>
+        <c:axId val="68794624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="68792704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="15"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>No. of Missions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68794624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="68794624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Value</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (science/$M)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.3944872059531885E-2"/>
+              <c:y val="0.19899356140118937"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68792704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1126,16 +1555,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>142876</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1158,16 +1587,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>133351</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1183,6 +1612,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1478,10 +1971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:M76"/>
+  <dimension ref="A4:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="O67" sqref="O67"/>
+    <sheetView tabSelected="1" topLeftCell="B51" workbookViewId="0">
+      <selection activeCell="N81" sqref="N81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,6 +1989,9 @@
     <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" customWidth="1"/>
     <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
@@ -1804,15 +2300,15 @@
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19" t="s">
+      <c r="C15" s="19"/>
+      <c r="D15" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
       <c r="I15" s="16">
         <v>2.6461999999999998E-5</v>
       </c>
@@ -2036,15 +2532,15 @@
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="19" t="s">
+      <c r="C38" s="19"/>
+      <c r="D38" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
       <c r="H38" s="2">
         <v>3</v>
       </c>
@@ -2100,7 +2596,7 @@
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>49</v>
       </c>
@@ -2113,8 +2609,17 @@
       <c r="M49" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O49" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>0</v>
       </c>
@@ -2141,8 +2646,17 @@
       <c r="M50" s="3">
         <v>3.3074000000000002E-5</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O50" s="5">
+        <v>10000</v>
+      </c>
+      <c r="P50" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q50" s="6">
+        <v>3.3074000000000002E-5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -2172,8 +2686,17 @@
       <c r="M51" s="3">
         <v>3.3074000000000002E-5</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O51" s="5">
+        <v>7140</v>
+      </c>
+      <c r="P51" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>4.5979000000000001E-5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2203,8 +2726,17 @@
       <c r="M52" s="3">
         <v>2.19E-5</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O52" s="5">
+        <v>1600</v>
+      </c>
+      <c r="P52" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q52" s="6">
+        <v>1.9023E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2235,8 +2767,8 @@
         <v>4.5979000000000001E-5</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="20">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" s="18">
         <v>7140</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -2266,8 +2798,8 @@
         <v>4.5969E-5</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="20">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" s="18">
         <v>7140</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -2297,8 +2829,8 @@
         <v>2.9509000000000002E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="20">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" s="18">
         <v>7140</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -2328,8 +2860,8 @@
         <v>1.9023E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="20">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="18">
         <v>1600</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -2359,8 +2891,8 @@
         <v>1.9023E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="20">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="18">
         <v>1600</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -2390,8 +2922,8 @@
         <v>1.9023E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="20">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="18">
         <v>1600</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -2410,18 +2942,18 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B60" s="18" t="s">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B60" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C60" s="18"/>
-      <c r="D60" s="19" t="s">
+      <c r="C60" s="19"/>
+      <c r="D60" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>55</v>
       </c>
@@ -2434,8 +2966,17 @@
       <c r="M65" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O65" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P65" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
         <v>0</v>
       </c>
@@ -2462,9 +3003,18 @@
       <c r="M66" s="3">
         <v>3.3074000000000002E-5</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" s="20">
+      <c r="O66" s="5">
+        <v>5</v>
+      </c>
+      <c r="P66" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q66" s="6">
+        <v>3.2468999999999997E-5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" s="18">
         <v>10</v>
       </c>
       <c r="B67" s="5" t="s">
@@ -2493,9 +3043,18 @@
       <c r="M67" s="3">
         <v>3.3074000000000002E-5</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="20">
+      <c r="O67" s="5">
+        <v>10</v>
+      </c>
+      <c r="P67" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q67" s="6">
+        <v>3.3074000000000002E-5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" s="18">
         <v>10</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -2524,9 +3083,18 @@
       <c r="M68" s="3">
         <v>2.19E-5</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="20">
+      <c r="O68" s="5">
+        <v>15</v>
+      </c>
+      <c r="P68" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q68" s="6">
+        <v>3.3352999999999997E-5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" s="18">
         <v>10</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -2556,8 +3124,8 @@
         <v>3.2468999999999997E-5</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A70" s="20">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70" s="18">
         <v>5</v>
       </c>
       <c r="B70" s="5" t="s">
@@ -2587,8 +3155,8 @@
         <v>3.2468999999999997E-5</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" s="20">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" s="18">
         <v>5</v>
       </c>
       <c r="B71" s="5" t="s">
@@ -2618,8 +3186,8 @@
         <v>1.9938000000000001E-5</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="20">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" s="18">
         <v>5</v>
       </c>
       <c r="B72" s="5" t="s">
@@ -2649,8 +3217,8 @@
         <v>3.3352999999999997E-5</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="20">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73" s="18">
         <v>15</v>
       </c>
       <c r="B73" s="5" t="s">
@@ -2680,8 +3248,8 @@
         <v>3.3352999999999997E-5</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" s="20">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" s="18">
         <v>15</v>
       </c>
       <c r="B74" s="5" t="s">
@@ -2711,8 +3279,8 @@
         <v>2.2751999999999998E-5</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="20">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A75" s="18">
         <v>15</v>
       </c>
       <c r="B75" s="5" t="s">
@@ -2731,17 +3299,17 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="20"/>
-      <c r="B76" s="18" t="s">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" s="18"/>
+      <c r="B76" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="18"/>
-      <c r="D76" s="19" t="s">
+      <c r="C76" s="19"/>
+      <c r="D76" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E76" s="19"/>
-      <c r="F76" s="19"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>